<commit_message>
Add example of using a time series
</commit_message>
<xml_diff>
--- a/docs/tutorials/extension.xlsx
+++ b/docs/tutorials/extension.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -443,7 +443,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t xml:space="preserve">Annualised capital costs</t>
   </si>
@@ -613,6 +613,9 @@
     <t xml:space="preserve">Time series ID</t>
   </si>
   <si>
+    <t xml:space="preserve">GridPrice</t>
+  </si>
+  <si>
     <t xml:space="preserve">Demand</t>
   </si>
   <si>
@@ -626,6 +629,9 @@
   </si>
   <si>
     <t xml:space="preserve">kW/m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$</t>
   </si>
   <si>
     <t xml:space="preserve">Data</t>
@@ -1152,7 +1158,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="1" sqref="E31 E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1206,7 +1212,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="E31 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1307,7 +1313,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="E31 H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1423,8 +1429,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="E31 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1719,7 +1725,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="1" sqref="E31 D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1871,10 +1877,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1896,24 +1902,30 @@
       <c r="D1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>17</v>
@@ -1923,11 +1935,14 @@
       </c>
       <c r="D3" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1941,17 +1956,20 @@
         <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>3</v>
@@ -1961,6 +1979,9 @@
       </c>
       <c r="D10" s="7" t="n">
         <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,6 +1994,9 @@
       <c r="D11" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
@@ -1984,6 +2008,9 @@
       <c r="D12" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
@@ -1995,6 +2022,9 @@
       <c r="D13" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E13" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
@@ -2006,6 +2036,9 @@
       <c r="D14" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -2017,6 +2050,9 @@
       <c r="D15" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
@@ -2028,6 +2064,9 @@
       <c r="D16" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
@@ -2039,6 +2078,9 @@
       <c r="D17" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
@@ -2050,6 +2092,9 @@
       <c r="D18" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
@@ -2061,6 +2106,9 @@
       <c r="D19" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E19" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
@@ -2072,6 +2120,9 @@
       <c r="D20" s="7" t="n">
         <v>56</v>
       </c>
+      <c r="E20" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
@@ -2083,6 +2134,9 @@
       <c r="D21" s="7" t="n">
         <v>192</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
@@ -2094,6 +2148,9 @@
       <c r="D22" s="7" t="n">
         <v>324</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
@@ -2105,6 +2162,9 @@
       <c r="D23" s="7" t="n">
         <v>380</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
@@ -2116,6 +2176,9 @@
       <c r="D24" s="7" t="n">
         <v>324</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
@@ -2127,6 +2190,9 @@
       <c r="D25" s="7" t="n">
         <v>189</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
@@ -2138,6 +2204,9 @@
       <c r="D26" s="7" t="n">
         <v>37</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
@@ -2149,6 +2218,9 @@
       <c r="D27" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
@@ -2160,6 +2232,9 @@
       <c r="D28" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E28" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
@@ -2171,6 +2246,9 @@
       <c r="D29" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E29" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="n">
@@ -2182,6 +2260,9 @@
       <c r="D30" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="n">
@@ -2193,6 +2274,9 @@
       <c r="D31" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E31" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
@@ -2204,6 +2288,9 @@
       <c r="D32" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="E32" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
@@ -2214,6 +2301,9 @@
       </c>
       <c r="D33" s="7" t="n">
         <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10972,7 +11062,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="E31 D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10989,12 +11079,12 @@
         <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
@@ -11060,7 +11150,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E31 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11071,37 +11161,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -11124,7 +11214,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+      <selection pane="topLeft" activeCell="F41" activeCellId="1" sqref="E31 F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11135,62 +11225,62 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>